<commit_message>
map for mycat to LVIS_cat
</commit_message>
<xml_diff>
--- a/dataset/LVIS/mycat_lvis_map.xlsx
+++ b/dataset/LVIS/mycat_lvis_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anranxu/Documents/lvis-api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anranxu/Documents/IUI_dataset/dataset/LVIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A63CA9-3D37-544F-A4D5-AABAACE2DE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{707817D2-44A4-0E48-B0DB-ED86687B6C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{B816A1BB-3749-B04D-A0AD-FA9D3F4B8A29}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{B816A1BB-3749-B04D-A0AD-FA9D3F4B8A29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>My Category</t>
     <phoneticPr fontId="1"/>
@@ -51,13 +51,82 @@
   </si>
   <si>
     <t>place identifier</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>Home interior</t>
+  </si>
+  <si>
+    <t>Vehicle Plate</t>
+  </si>
+  <si>
+    <t>Bystander</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Paper/Document/Label</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Scenery</t>
+  </si>
+  <si>
+    <t>Pet</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Electronic devices</t>
+  </si>
+  <si>
+    <t>Toiletries</t>
+  </si>
+  <si>
+    <t>Toy</t>
+  </si>
+  <si>
+    <t>Finger</t>
+  </si>
+  <si>
+    <t>Cigarettes</t>
+  </si>
+  <si>
+    <t>Accident</t>
+  </si>
+  <si>
+    <t>Music instrument</t>
+  </si>
+  <si>
+    <t>Nudity</t>
+  </si>
+  <si>
+    <t>Accessory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -70,6 +139,14 @@
       <sz val="6"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -96,8 +173,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CEA9DB-77C7-B343-B64C-6C5F3628448E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -447,6 +527,121 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>